<commit_message>
Version3: Thanusha PR Comments
</commit_message>
<xml_diff>
--- a/CTS-SAT-1 Onboard Computer/Project Outputs for OBC Development Board/OBC Development Board.xlsx
+++ b/CTS-SAT-1 Onboard Computer/Project Outputs for OBC Development Board/OBC Development Board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sixtium\Documents\GitStuff\CTS-SAT-1-OBC-PCB\CTS-SAT-1 Onboard Computer\Project Outputs for OBC Development Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B224346F-B036-4E51-9E48-C6D35FFA5C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5842A973-B1B3-4F94-845F-A9EC5988A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{F42A7DC2-DE70-4DA9-BDE0-809696854082}"/>
+    <workbookView xWindow="6468" yWindow="4452" windowWidth="11076" windowHeight="5736" xr2:uid="{1C25B0C8-E5B5-4D3C-953D-ACC663597178}"/>
   </bookViews>
   <sheets>
     <sheet name="OBC Development Board" sheetId="1" r:id="rId1"/>
@@ -311,7 +311,7 @@
     <t>RR0816P-221-D</t>
   </si>
   <si>
-    <t>R4, R5, R6, R7, R13, R14, R15, R16, R17, R22, R24, R26, R27, R28, R30, R31, R32, R33, R34, R35, R36, R37, R38, R41, R42, R43, R44, R45, R46, R47, R51, R52, R53, R55, R63, R64, R67, R107, R109</t>
+    <t>R4, R5, R6, R7, R13, R14, R15, R16, R17, R22, R24, R26, R27, R28, R30, R31, R32, R33, R34, R35, R36, R37, R38, R41, R42, R43, R44, R45, R46, R47, R51, R52, R53, R55, R63, R64, R67, R68, R69, R107, R109</t>
   </si>
   <si>
     <t>0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
@@ -939,7 +939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCD3CF9-B0BC-43EF-A431-39C0056F6546}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791A4FB0-6BC6-4C75-A215-96E1BAA30FAF}">
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1402,7 +1402,7 @@
         <v>93</v>
       </c>
       <c r="E26" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1780,6 +1780,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version3: Working on components
</commit_message>
<xml_diff>
--- a/CTS-SAT-1 Onboard Computer/Project Outputs for OBC Development Board/OBC Development Board.xlsx
+++ b/CTS-SAT-1 Onboard Computer/Project Outputs for OBC Development Board/OBC Development Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sixtium\Documents\GitStuff\CTS-SAT-1-OBC-PCB\CTS-SAT-1 Onboard Computer\Project Outputs for OBC Development Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5842A973-B1B3-4F94-845F-A9EC5988A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9536CC3-FD2A-44BC-8334-95370EBD3145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6468" yWindow="4452" windowWidth="11076" windowHeight="5736" xr2:uid="{1C25B0C8-E5B5-4D3C-953D-ACC663597178}"/>
+    <workbookView xWindow="35820" yWindow="4785" windowWidth="11070" windowHeight="5730" xr2:uid="{4F5AFCB7-DC5B-41D0-8DBE-59532CE56E48}"/>
   </bookViews>
   <sheets>
     <sheet name="OBC Development Board" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="216">
   <si>
     <t>Designator</t>
   </si>
@@ -56,7 +56,16 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>LCSC Part #</t>
+    <t>Distrbutor</t>
+  </si>
+  <si>
+    <t>Distrbutor part #</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t>Distributor Part #</t>
   </si>
   <si>
     <t>*1, *2, *3, *4</t>
@@ -77,6 +86,12 @@
     <t>CL10B104KA8NNNC</t>
   </si>
   <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>1276-1006-1-ND</t>
+  </si>
+  <si>
     <t>C2, C31</t>
   </si>
   <si>
@@ -89,6 +104,9 @@
     <t>CC0603KRX7R8BB105</t>
   </si>
   <si>
+    <t>311-1802-1-ND</t>
+  </si>
+  <si>
     <t>C11, C13, C48, C49, C50</t>
   </si>
   <si>
@@ -101,6 +119,9 @@
     <t>TAJA475K020RNJ</t>
   </si>
   <si>
+    <t>478-1668-1-ND</t>
+  </si>
+  <si>
     <t>C12, C20, C52, C54</t>
   </si>
   <si>
@@ -113,6 +134,9 @@
     <t>CC0402KPX7R8BB104</t>
   </si>
   <si>
+    <t>13-CC0402KPX7R8BB104CT-ND</t>
+  </si>
+  <si>
     <t>C21</t>
   </si>
   <si>
@@ -122,6 +146,9 @@
     <t>CC0402FRNPO9BN150</t>
   </si>
   <si>
+    <t>311-1642-1-ND</t>
+  </si>
+  <si>
     <t>C33</t>
   </si>
   <si>
@@ -134,6 +161,9 @@
     <t>TPSA226K010T0900</t>
   </si>
   <si>
+    <t>478-11193-1-ND</t>
+  </si>
+  <si>
     <t>C34, C35, C36</t>
   </si>
   <si>
@@ -146,6 +176,9 @@
     <t>25SVPF47M</t>
   </si>
   <si>
+    <t>P16513CT-ND</t>
+  </si>
+  <si>
     <t>C37, C38, C40, C41</t>
   </si>
   <si>
@@ -158,6 +191,9 @@
     <t>CBR06C708B5GAC</t>
   </si>
   <si>
+    <t>399-CBR06C708B5GACCT-ND</t>
+  </si>
+  <si>
     <t>C39, C44</t>
   </si>
   <si>
@@ -170,6 +206,9 @@
     <t>GRM188Z71C475KE21J</t>
   </si>
   <si>
+    <t>490-GRM188Z71C475KE21JCT-ND</t>
+  </si>
+  <si>
     <t>C42, C45, C47</t>
   </si>
   <si>
@@ -179,6 +218,9 @@
     <t>CC0603KRX7R9BB101</t>
   </si>
   <si>
+    <t>311-3601-1-ND</t>
+  </si>
+  <si>
     <t>C43, C46</t>
   </si>
   <si>
@@ -188,6 +230,9 @@
     <t>C0603C330K5RAC7867</t>
   </si>
   <si>
+    <t>399-C0603C330K5RAC7867CT-ND</t>
+  </si>
+  <si>
     <t>D1, D2, D3, D4, D5, D6</t>
   </si>
   <si>
@@ -200,6 +245,9 @@
     <t>SML-D12U1WT86</t>
   </si>
   <si>
+    <t>SML-D12U1WT86CT-ND</t>
+  </si>
+  <si>
     <t>D7</t>
   </si>
   <si>
@@ -212,6 +260,9 @@
     <t>B540C-13-F</t>
   </si>
   <si>
+    <t>B540C-FDICT-ND</t>
+  </si>
+  <si>
     <t>J1, J2, J15, J19, J21</t>
   </si>
   <si>
@@ -224,18 +275,33 @@
     <t>TSW-106-05-T-S</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>SAM12323-ND</t>
+  </si>
+  <si>
     <t>J3, J8</t>
   </si>
   <si>
     <t>CONN HEADER SMD R/A 8POS 1.25MM</t>
   </si>
   <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>WM7626CT-ND</t>
+  </si>
+  <si>
     <t>J4</t>
   </si>
   <si>
     <t>CONN HEADER SMD R/A 4POS 1.25MM</t>
   </si>
   <si>
+    <t>WM7622CT-ND</t>
+  </si>
+  <si>
     <t>J5, J6</t>
   </si>
   <si>
@@ -248,12 +314,18 @@
     <t>ESQ-126-14-G-D</t>
   </si>
   <si>
+    <t>SAM11114-ND</t>
+  </si>
+  <si>
     <t>J7, J9, J11</t>
   </si>
   <si>
     <t>CONN HEADER SMD R/A 6POS 1.25MM</t>
   </si>
   <si>
+    <t>WM7624CT-ND</t>
+  </si>
+  <si>
     <t>J10, J13</t>
   </si>
   <si>
@@ -266,6 +338,9 @@
     <t>0530471010</t>
   </si>
   <si>
+    <t>WM1739-ND</t>
+  </si>
+  <si>
     <t>J12</t>
   </si>
   <si>
@@ -275,6 +350,9 @@
     <t>0532617014</t>
   </si>
   <si>
+    <t>900-0532617014CT-ND</t>
+  </si>
+  <si>
     <t>J14, J16, J17, J18, J20</t>
   </si>
   <si>
@@ -287,6 +365,9 @@
     <t>252105</t>
   </si>
   <si>
+    <t>ACX1262-ND</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -299,6 +380,9 @@
     <t>IHLP4040DZER6R8M01</t>
   </si>
   <si>
+    <t>541-1303-1-ND</t>
+  </si>
+  <si>
     <t>R1, R2, R3, R134, R135</t>
   </si>
   <si>
@@ -311,6 +395,9 @@
     <t>RR0816P-221-D</t>
   </si>
   <si>
+    <t>RR08P220DCT-ND</t>
+  </si>
+  <si>
     <t>R4, R5, R6, R7, R13, R14, R15, R16, R17, R22, R24, R26, R27, R28, R30, R31, R32, R33, R34, R35, R36, R37, R38, R41, R42, R43, R44, R45, R46, R47, R51, R52, R53, R55, R63, R64, R67, R68, R69, R107, R109</t>
   </si>
   <si>
@@ -323,6 +410,9 @@
     <t>RMCF0603ZT0R00</t>
   </si>
   <si>
+    <t>RMCF0603ZT0R00CT-ND</t>
+  </si>
+  <si>
     <t>R8, R11</t>
   </si>
   <si>
@@ -335,6 +425,9 @@
     <t>CPF0603F1K0C1</t>
   </si>
   <si>
+    <t>A102226CT-ND</t>
+  </si>
+  <si>
     <t>R9, R10, R12, R18, R21, R23, R25, R29, R39, R40, R48, R50, R56, R57, R58, R59</t>
   </si>
   <si>
@@ -344,6 +437,9 @@
     <t>RR0816Q-220-D</t>
   </si>
   <si>
+    <t>RR08Q22DCT-ND</t>
+  </si>
+  <si>
     <t>R19, R20, R49, R54, R91, R92</t>
   </si>
   <si>
@@ -356,6 +452,9 @@
     <t>CR0603-FX-4701ELF</t>
   </si>
   <si>
+    <t>CR0603-FX-4701ELFCT-ND</t>
+  </si>
+  <si>
     <t>R60, R61, R65, R66, R117, R118, R119, R120, R124, R125, R126, R127, R128, R129, R136</t>
   </si>
   <si>
@@ -368,6 +467,9 @@
     <t>RNCP0603FTD10K0, CPF0603B10KE</t>
   </si>
   <si>
+    <t>RNCP0603FTD10K0CT-ND, A119886CT-ND</t>
+  </si>
+  <si>
     <t>R62</t>
   </si>
   <si>
@@ -377,6 +479,12 @@
     <t>WSR2R2500FEA</t>
   </si>
   <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>C4299447</t>
+  </si>
+  <si>
     <t>R130, R131</t>
   </si>
   <si>
@@ -419,7 +527,7 @@
     <t>STM32L4R5ZIT6</t>
   </si>
   <si>
-    <t>C1339786</t>
+    <t>Mouser</t>
   </si>
   <si>
     <t>U2, U3, U5, U6</t>
@@ -434,7 +542,7 @@
     <t>S70FL01GSAGMFI011</t>
   </si>
   <si>
-    <t>C476475</t>
+    <t>1274-1092-ND</t>
   </si>
   <si>
     <t>U4</t>
@@ -449,6 +557,9 @@
     <t>ADP2303ARDZ</t>
   </si>
   <si>
+    <t>505-ADP2303ARDZ-ND</t>
+  </si>
+  <si>
     <t>U7, U8</t>
   </si>
   <si>
@@ -458,6 +569,9 @@
     <t>CY15B108QN-40LPXI</t>
   </si>
   <si>
+    <t>428-4723-ND</t>
+  </si>
+  <si>
     <t>U9</t>
   </si>
   <si>
@@ -470,7 +584,7 @@
     <t>MAX3378EEUD+T</t>
   </si>
   <si>
-    <t>C143441</t>
+    <t>MAX3378EEUD+TCT-ND</t>
   </si>
   <si>
     <t>U10</t>
@@ -485,7 +599,7 @@
     <t>MAX3086EESD+T</t>
   </si>
   <si>
-    <t>C2671104</t>
+    <t>MAX3086EESD+TCT-ND</t>
   </si>
   <si>
     <t>U11, U12</t>
@@ -500,6 +614,9 @@
     <t>317990829</t>
   </si>
   <si>
+    <t>1597-317990829CT-ND</t>
+  </si>
+  <si>
     <t>U13</t>
   </si>
   <si>
@@ -527,7 +644,7 @@
     <t>SN74LVC1G14DCKR</t>
   </si>
   <si>
-    <t>C35740</t>
+    <t>296-11608-1-ND</t>
   </si>
   <si>
     <t>U15</t>
@@ -554,6 +671,9 @@
     <t>ECS-TXO-2520-33-250-AN-TR</t>
   </si>
   <si>
+    <t>XC2258CT-ND</t>
+  </si>
+  <si>
     <t>Y2</t>
   </si>
   <si>
@@ -564,6 +684,9 @@
   </si>
   <si>
     <t>TG-3541CE 32.7680KXB3</t>
+  </si>
+  <si>
+    <t>SER4422CT-ND</t>
   </si>
 </sst>
 </file>
@@ -939,20 +1062,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791A4FB0-6BC6-4C75-A215-96E1BAA30FAF}">
-  <dimension ref="A1:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40B7566-69E0-48F8-BD53-F99E783FB38B}">
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="1" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -971,13 +1091,22 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -985,265 +1114,366 @@
         <v>4</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>27</v>
       </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1"/>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1"/>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1"/>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1"/>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1"/>
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="1"/>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="1"/>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="1"/>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1">
         <v>6</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="1"/>
+      <c r="H14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="1"/>
+      <c r="H15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1">
         <v>5</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1251,13 +1481,20 @@
         <v>2</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+      <c r="H17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1265,31 +1502,45 @@
         <v>1</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="H18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="1"/>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1297,249 +1548,345 @@
         <v>3</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="1"/>
+      <c r="H20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="1"/>
+      <c r="H21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="1"/>
+      <c r="H22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="E23" s="1">
         <v>5</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="1"/>
+      <c r="H23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
       </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="1"/>
+      <c r="H24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1">
         <v>5</v>
       </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="1"/>
+      <c r="H25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="E26" s="1">
         <v>41</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="1"/>
+      <c r="H26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
       </c>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="1"/>
+      <c r="H27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="E28" s="1">
         <v>16</v>
       </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="1"/>
+      <c r="H28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1">
         <v>6</v>
       </c>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="1"/>
+      <c r="H29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="E30" s="1">
         <v>15</v>
       </c>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="1"/>
+      <c r="H30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="1"/>
+      <c r="H31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="E32" s="1">
         <v>2</v>
       </c>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="1"/>
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1547,236 +1894,307 @@
         <v>2</v>
       </c>
       <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
       </c>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="1"/>
+      <c r="H37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="E38" s="1">
         <v>2</v>
       </c>
       <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="1"/>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
       </c>
       <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="1"/>
+      <c r="H41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>156</v>
+        <v>195</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
       </c>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="1"/>
+      <c r="H45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
       </c>
       <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>